<commit_message>
added dynamic factor for k_c
</commit_message>
<xml_diff>
--- a/example/result.xlsx
+++ b/example/result.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="72">
   <si>
     <t>init</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>Rail_Relative_Number_of_Rolling_Contacts v_c</t>
+  </si>
+  <si>
+    <t>Dynamic_Factor</t>
   </si>
   <si>
     <t>W250-FL</t>
@@ -654,7 +657,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -818,22 +821,22 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -843,13 +846,13 @@
         <v>25</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -859,13 +862,13 @@
         <v>26</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -875,13 +878,13 @@
         <v>27</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1046,36 +1049,36 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="5"/>
-      <c r="B24" s="7" t="s">
-        <v>69</v>
-      </c>
+      <c r="B24" s="6"/>
       <c r="C24" s="4" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="D24" s="2">
-        <v>24.9397924881983</v>
+        <v>1.1</v>
       </c>
       <c r="E24" s="2">
-        <v>29.8460335067485</v>
+        <v>1</v>
       </c>
       <c r="F24" s="2">
-        <v>29.8460335067485</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="5"/>
-      <c r="B25" s="7"/>
+      <c r="B25" s="7" t="s">
+        <v>70</v>
+      </c>
       <c r="C25" s="4" t="s">
         <v>50</v>
       </c>
       <c r="D25" s="2">
-        <v>0.397534327540081</v>
+        <v>24.9397924881983</v>
       </c>
       <c r="E25" s="2">
-        <v>0.387456729691634</v>
+        <v>29.8460335067485</v>
       </c>
       <c r="F25" s="2">
-        <v>0.387456729691634</v>
+        <v>29.8460335067485</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1085,13 +1088,13 @@
         <v>51</v>
       </c>
       <c r="D26" s="2">
-        <v>310.534232585119</v>
+        <v>0.397534327540081</v>
       </c>
       <c r="E26" s="2">
-        <v>311.826319322442</v>
+        <v>0.387456729691634</v>
       </c>
       <c r="F26" s="2">
-        <v>311.826319322442</v>
+        <v>0.387456729691634</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1101,13 +1104,13 @@
         <v>52</v>
       </c>
       <c r="D27" s="2">
-        <v>0.2</v>
+        <v>310.534232585119</v>
       </c>
       <c r="E27" s="2">
-        <v>0.278960201647951</v>
+        <v>311.826319322442</v>
       </c>
       <c r="F27" s="2">
-        <v>0.278960201647951</v>
+        <v>311.826319322442</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1117,13 +1120,13 @@
         <v>53</v>
       </c>
       <c r="D28" s="2">
-        <v>9592.88212951047</v>
+        <v>0.2</v>
       </c>
       <c r="E28" s="2">
-        <v>13728.6250951821</v>
+        <v>0.278960201647951</v>
       </c>
       <c r="F28" s="2">
-        <v>13728.6250951821</v>
+        <v>0.278960201647951</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1133,13 +1136,13 @@
         <v>54</v>
       </c>
       <c r="D29" s="2">
-        <v>6.98593533053798</v>
+        <v>9592.88212951047</v>
       </c>
       <c r="E29" s="2">
-        <v>4.86670380638896</v>
+        <v>13728.6250951821</v>
       </c>
       <c r="F29" s="2">
-        <v>4.86670380638896</v>
+        <v>13728.6250951821</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1149,13 +1152,13 @@
         <v>55</v>
       </c>
       <c r="D30" s="2">
-        <v>0.360322324557323</v>
+        <v>6.98593533053798</v>
       </c>
       <c r="E30" s="2">
-        <v>0.432635531364102</v>
+        <v>4.86670380638896</v>
       </c>
       <c r="F30" s="2">
-        <v>0.432635531364102</v>
+        <v>4.86670380638896</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1165,13 +1168,13 @@
         <v>56</v>
       </c>
       <c r="D31" s="2">
-        <v>235.360704664796</v>
+        <v>0.360322324557323</v>
       </c>
       <c r="E31" s="2">
-        <v>208.806759033595</v>
+        <v>0.432635531364102</v>
       </c>
       <c r="F31" s="2">
-        <v>208.806759033595</v>
+        <v>0.432635531364102</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1181,13 +1184,13 @@
         <v>57</v>
       </c>
       <c r="D32" s="2">
-        <v>3620.84483241631</v>
+        <v>235.360704664796</v>
       </c>
       <c r="E32" s="2">
-        <v>2311.15858694705</v>
+        <v>208.806759033595</v>
       </c>
       <c r="F32" s="2">
-        <v>2311.15858694705</v>
+        <v>208.806759033595</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1197,13 +1200,13 @@
         <v>58</v>
       </c>
       <c r="D33" s="2">
-        <v>1.13373577673032</v>
+        <v>3620.84483241631</v>
       </c>
       <c r="E33" s="2">
-        <v>2.42581799694202</v>
+        <v>2311.15858694705</v>
       </c>
       <c r="F33" s="2">
-        <v>2.42581799694202</v>
+        <v>2311.15858694705</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1213,13 +1216,13 @@
         <v>59</v>
       </c>
       <c r="D34" s="2">
-        <v>0.675758774397529</v>
+        <v>1.13373577673032</v>
       </c>
       <c r="E34" s="2">
-        <v>0.517120004340175</v>
+        <v>2.42581799694202</v>
       </c>
       <c r="F34" s="2">
-        <v>0.517120004340175</v>
+        <v>2.42581799694202</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1229,13 +1232,13 @@
         <v>60</v>
       </c>
       <c r="D35" s="2">
-        <v>3.8387980542433</v>
+        <v>0.675758774397529</v>
       </c>
       <c r="E35" s="2">
-        <v>1.87763390038708</v>
+        <v>0.517120004340175</v>
       </c>
       <c r="F35" s="2">
-        <v>1.87763390038708</v>
+        <v>0.517120004340175</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1245,13 +1248,13 @@
         <v>61</v>
       </c>
       <c r="D36" s="2">
-        <v>1.2</v>
+        <v>3.8387980542433</v>
       </c>
       <c r="E36" s="2">
-        <v>3.2</v>
+        <v>1.87763390038708</v>
       </c>
       <c r="F36" s="2">
-        <v>3.1</v>
+        <v>1.87763390038708</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1261,13 +1264,13 @@
         <v>62</v>
       </c>
       <c r="D37" s="2">
-        <v>2351.03585576092</v>
+        <v>1.2</v>
       </c>
       <c r="E37" s="2">
-        <v>2600</v>
+        <v>3.2</v>
       </c>
       <c r="F37" s="2">
-        <v>2600</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1277,13 +1280,13 @@
         <v>63</v>
       </c>
       <c r="D38" s="2">
-        <v>479.564279785433</v>
+        <v>2351.03585576092</v>
       </c>
       <c r="E38" s="2">
-        <v>342.07526272382</v>
+        <v>2600</v>
       </c>
       <c r="F38" s="2">
-        <v>342.07526272382</v>
+        <v>2600</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1293,13 +1296,13 @@
         <v>64</v>
       </c>
       <c r="D39" s="2">
-        <v>1.5209241133552</v>
+        <v>479.564279785433</v>
       </c>
       <c r="E39" s="2">
-        <v>1.4611356146706</v>
+        <v>342.07526272382</v>
       </c>
       <c r="F39" s="2">
-        <v>1.4611356146706</v>
+        <v>342.07526272382</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1309,13 +1312,13 @@
         <v>65</v>
       </c>
       <c r="D40" s="2">
-        <v>148.023377589456</v>
+        <v>1.5209241133552</v>
       </c>
       <c r="E40" s="2">
-        <v>90</v>
+        <v>1.4611356146706</v>
       </c>
       <c r="F40" s="2">
-        <v>90</v>
+        <v>1.4611356146706</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1325,13 +1328,13 @@
         <v>66</v>
       </c>
       <c r="D41" s="2">
-        <v>4000000</v>
+        <v>148.023377589456</v>
       </c>
       <c r="E41" s="2">
-        <v>4000000</v>
+        <v>90</v>
       </c>
       <c r="F41" s="2">
-        <v>4000000</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1341,13 +1344,13 @@
         <v>67</v>
       </c>
       <c r="D42" s="2">
-        <v>12000000</v>
+        <v>4000000</v>
       </c>
       <c r="E42" s="2">
-        <v>13000000</v>
+        <v>4000000</v>
       </c>
       <c r="F42" s="2">
-        <v>13000000</v>
+        <v>4000000</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1357,12 +1360,28 @@
         <v>68</v>
       </c>
       <c r="D43" s="2">
+        <v>12000000</v>
+      </c>
+      <c r="E43" s="2">
+        <v>13000000</v>
+      </c>
+      <c r="F43" s="2">
+        <v>13000000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="5"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D44" s="2">
         <v>1</v>
       </c>
-      <c r="E43" s="2">
+      <c r="E44" s="2">
         <v>2</v>
       </c>
-      <c r="F43" s="2">
+      <c r="F44" s="2">
         <v>4</v>
       </c>
     </row>
@@ -1372,9 +1391,9 @@
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="A1:A9"/>
-    <mergeCell ref="B10:B23"/>
-    <mergeCell ref="B24:B43"/>
-    <mergeCell ref="A10:A43"/>
+    <mergeCell ref="B10:B24"/>
+    <mergeCell ref="B25:B44"/>
+    <mergeCell ref="A10:A44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1382,7 +1401,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G76"/>
+  <dimension ref="A1:G77"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1501,7 +1520,7 @@
         <v>12</v>
       </c>
       <c r="D7" s="2">
-        <v>0.4173026084899902</v>
+        <v>0.4590328693389893</v>
       </c>
       <c r="E7" s="2">
         <v>0.06757307052612305</v>
@@ -1517,7 +1536,7 @@
         <v>13</v>
       </c>
       <c r="D8" s="2">
-        <v>49.84321962666694</v>
+        <v>54.82754158933363</v>
       </c>
       <c r="E8" s="2">
         <v>0.5405845642089844</v>
@@ -1533,7 +1552,7 @@
         <v>14</v>
       </c>
       <c r="D9" s="2">
-        <v>24.90150727043514</v>
+        <v>24.19958007275333</v>
       </c>
       <c r="E9" s="2">
         <v>136.0655020108048</v>
@@ -1565,7 +1584,7 @@
         <v>16</v>
       </c>
       <c r="D11" s="2">
-        <v>0.4468460381031036</v>
+        <v>0.491530641913414</v>
       </c>
       <c r="E11" s="2">
         <v>0.1163399890065193</v>
@@ -1581,7 +1600,7 @@
         <v>17</v>
       </c>
       <c r="D12" s="2">
-        <v>53.3719290590373</v>
+        <v>58.70912196494103</v>
       </c>
       <c r="E12" s="2">
         <v>0.9307199120521544</v>
@@ -1597,7 +1616,7 @@
         <v>18</v>
       </c>
       <c r="D13" s="2">
-        <v>24.39571728216994</v>
+        <v>23.70804736398622</v>
       </c>
       <c r="E13" s="2">
         <v>115.6009542115067</v>
@@ -1731,7 +1750,7 @@
         <v>12</v>
       </c>
       <c r="D21" s="2">
-        <v>0.1661300659179688</v>
+        <v>0.1827430725097657</v>
       </c>
       <c r="E21" s="2">
         <v>0.0281226634979248</v>
@@ -1747,7 +1766,7 @@
         <v>13</v>
       </c>
       <c r="D22" s="2">
-        <v>19.84281237087113</v>
+        <v>21.82709360795825</v>
       </c>
       <c r="E22" s="2">
         <v>0.2249813079833984</v>
@@ -1763,7 +1782,7 @@
         <v>14</v>
       </c>
       <c r="D23" s="2">
-        <v>32.82664465837629</v>
+        <v>31.90132257067649</v>
       </c>
       <c r="E23" s="2">
         <v>176.9958930844957</v>
@@ -1795,7 +1814,7 @@
         <v>16</v>
       </c>
       <c r="D25" s="2">
-        <v>0.1908901929855347</v>
+        <v>0.2099792122840881</v>
       </c>
       <c r="E25" s="2">
         <v>0.06478920578956604</v>
@@ -1811,7 +1830,7 @@
         <v>17</v>
       </c>
       <c r="D26" s="2">
-        <v>22.80019731480558</v>
+        <v>25.08021704628614</v>
       </c>
       <c r="E26" s="2">
         <v>0.5183136463165283</v>
@@ -1827,7 +1846,7 @@
         <v>18</v>
       </c>
       <c r="D27" s="2">
-        <v>31.48660820406486</v>
+        <v>30.59905925286444</v>
       </c>
       <c r="E27" s="2">
         <v>137.7936891246582</v>
@@ -1961,7 +1980,7 @@
         <v>12</v>
       </c>
       <c r="D35" s="2">
-        <v>0.1979813575744629</v>
+        <v>0.2177794933319092</v>
       </c>
       <c r="E35" s="2">
         <v>0.03665781021118164</v>
@@ -1977,7 +1996,7 @@
         <v>13</v>
       </c>
       <c r="D36" s="2">
-        <v>1.484860181808471</v>
+        <v>1.633346199989319</v>
       </c>
       <c r="E36" s="2">
         <v>0.2978447079658508</v>
@@ -1993,7 +2012,7 @@
         <v>14</v>
       </c>
       <c r="D37" s="2">
-        <v>56.95944487714801</v>
+        <v>55.35386401451498</v>
       </c>
       <c r="E37" s="2">
         <v>129.7101939713239</v>
@@ -2025,7 +2044,7 @@
         <v>16</v>
       </c>
       <c r="D39" s="2">
-        <v>0.2761687934398651</v>
+        <v>0.3037856727838517</v>
       </c>
       <c r="E39" s="2">
         <v>0.1420809924602509</v>
@@ -2041,7 +2060,7 @@
         <v>17</v>
       </c>
       <c r="D40" s="2">
-        <v>2.071265950798988</v>
+        <v>2.278392545878888</v>
       </c>
       <c r="E40" s="2">
         <v>1.154408063739538</v>
@@ -2057,7 +2076,7 @@
         <v>18</v>
       </c>
       <c r="D41" s="2">
-        <v>51.54667501729854</v>
+        <v>50.09367007459512</v>
       </c>
       <c r="E41" s="2">
         <v>86.38995935762931</v>
@@ -2084,22 +2103,22 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -2109,13 +2128,13 @@
         <v>25</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -2125,13 +2144,13 @@
         <v>26</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -2141,13 +2160,13 @@
         <v>27</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -2312,36 +2331,36 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="5"/>
-      <c r="B57" s="7" t="s">
-        <v>69</v>
-      </c>
+      <c r="B57" s="6"/>
       <c r="C57" s="4" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="D57" s="2">
-        <v>24.9397924881983</v>
+        <v>1.1</v>
       </c>
       <c r="E57" s="2">
-        <v>29.8460335067485</v>
+        <v>1</v>
       </c>
       <c r="F57" s="2">
-        <v>29.8460335067485</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="5"/>
-      <c r="B58" s="7"/>
+      <c r="B58" s="7" t="s">
+        <v>70</v>
+      </c>
       <c r="C58" s="4" t="s">
         <v>50</v>
       </c>
       <c r="D58" s="2">
-        <v>0.397534327540081</v>
+        <v>24.9397924881983</v>
       </c>
       <c r="E58" s="2">
-        <v>0.387456729691634</v>
+        <v>29.8460335067485</v>
       </c>
       <c r="F58" s="2">
-        <v>0.387456729691634</v>
+        <v>29.8460335067485</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2351,13 +2370,13 @@
         <v>51</v>
       </c>
       <c r="D59" s="2">
-        <v>310.534232585119</v>
+        <v>0.397534327540081</v>
       </c>
       <c r="E59" s="2">
-        <v>311.826319322442</v>
+        <v>0.387456729691634</v>
       </c>
       <c r="F59" s="2">
-        <v>311.826319322442</v>
+        <v>0.387456729691634</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2367,13 +2386,13 @@
         <v>52</v>
       </c>
       <c r="D60" s="2">
-        <v>0.2</v>
+        <v>310.534232585119</v>
       </c>
       <c r="E60" s="2">
-        <v>0.278960201647951</v>
+        <v>311.826319322442</v>
       </c>
       <c r="F60" s="2">
-        <v>0.278960201647951</v>
+        <v>311.826319322442</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2383,13 +2402,13 @@
         <v>53</v>
       </c>
       <c r="D61" s="2">
-        <v>9592.88212951047</v>
+        <v>0.2</v>
       </c>
       <c r="E61" s="2">
-        <v>13728.6250951821</v>
+        <v>0.278960201647951</v>
       </c>
       <c r="F61" s="2">
-        <v>13728.6250951821</v>
+        <v>0.278960201647951</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2399,13 +2418,13 @@
         <v>54</v>
       </c>
       <c r="D62" s="2">
-        <v>6.98593533053798</v>
+        <v>9592.88212951047</v>
       </c>
       <c r="E62" s="2">
-        <v>4.86670380638896</v>
+        <v>13728.6250951821</v>
       </c>
       <c r="F62" s="2">
-        <v>4.86670380638896</v>
+        <v>13728.6250951821</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -2415,13 +2434,13 @@
         <v>55</v>
       </c>
       <c r="D63" s="2">
-        <v>0.360322324557323</v>
+        <v>6.98593533053798</v>
       </c>
       <c r="E63" s="2">
-        <v>0.432635531364102</v>
+        <v>4.86670380638896</v>
       </c>
       <c r="F63" s="2">
-        <v>0.432635531364102</v>
+        <v>4.86670380638896</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -2431,13 +2450,13 @@
         <v>56</v>
       </c>
       <c r="D64" s="2">
-        <v>235.360704664796</v>
+        <v>0.360322324557323</v>
       </c>
       <c r="E64" s="2">
-        <v>208.806759033595</v>
+        <v>0.432635531364102</v>
       </c>
       <c r="F64" s="2">
-        <v>208.806759033595</v>
+        <v>0.432635531364102</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -2447,13 +2466,13 @@
         <v>57</v>
       </c>
       <c r="D65" s="2">
-        <v>3620.84483241631</v>
+        <v>235.360704664796</v>
       </c>
       <c r="E65" s="2">
-        <v>2311.15858694705</v>
+        <v>208.806759033595</v>
       </c>
       <c r="F65" s="2">
-        <v>2311.15858694705</v>
+        <v>208.806759033595</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -2463,13 +2482,13 @@
         <v>58</v>
       </c>
       <c r="D66" s="2">
-        <v>1.13373577673032</v>
+        <v>3620.84483241631</v>
       </c>
       <c r="E66" s="2">
-        <v>2.42581799694202</v>
+        <v>2311.15858694705</v>
       </c>
       <c r="F66" s="2">
-        <v>2.42581799694202</v>
+        <v>2311.15858694705</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -2479,13 +2498,13 @@
         <v>59</v>
       </c>
       <c r="D67" s="2">
-        <v>0.675758774397529</v>
+        <v>1.13373577673032</v>
       </c>
       <c r="E67" s="2">
-        <v>0.517120004340175</v>
+        <v>2.42581799694202</v>
       </c>
       <c r="F67" s="2">
-        <v>0.517120004340175</v>
+        <v>2.42581799694202</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -2495,13 +2514,13 @@
         <v>60</v>
       </c>
       <c r="D68" s="2">
-        <v>3.8387980542433</v>
+        <v>0.675758774397529</v>
       </c>
       <c r="E68" s="2">
-        <v>1.87763390038708</v>
+        <v>0.517120004340175</v>
       </c>
       <c r="F68" s="2">
-        <v>1.87763390038708</v>
+        <v>0.517120004340175</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -2511,13 +2530,13 @@
         <v>61</v>
       </c>
       <c r="D69" s="2">
-        <v>1.2</v>
+        <v>3.8387980542433</v>
       </c>
       <c r="E69" s="2">
-        <v>3.2</v>
+        <v>1.87763390038708</v>
       </c>
       <c r="F69" s="2">
-        <v>3.1</v>
+        <v>1.87763390038708</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -2527,13 +2546,13 @@
         <v>62</v>
       </c>
       <c r="D70" s="2">
-        <v>2351.03585576092</v>
+        <v>1.2</v>
       </c>
       <c r="E70" s="2">
-        <v>2600</v>
+        <v>3.2</v>
       </c>
       <c r="F70" s="2">
-        <v>2600</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -2543,13 +2562,13 @@
         <v>63</v>
       </c>
       <c r="D71" s="2">
-        <v>479.564279785433</v>
+        <v>2351.03585576092</v>
       </c>
       <c r="E71" s="2">
-        <v>342.07526272382</v>
+        <v>2600</v>
       </c>
       <c r="F71" s="2">
-        <v>342.07526272382</v>
+        <v>2600</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2559,13 +2578,13 @@
         <v>64</v>
       </c>
       <c r="D72" s="2">
-        <v>1.5209241133552</v>
+        <v>479.564279785433</v>
       </c>
       <c r="E72" s="2">
-        <v>1.4611356146706</v>
+        <v>342.07526272382</v>
       </c>
       <c r="F72" s="2">
-        <v>1.4611356146706</v>
+        <v>342.07526272382</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2575,13 +2594,13 @@
         <v>65</v>
       </c>
       <c r="D73" s="2">
-        <v>148.023377589456</v>
+        <v>1.5209241133552</v>
       </c>
       <c r="E73" s="2">
-        <v>90</v>
+        <v>1.4611356146706</v>
       </c>
       <c r="F73" s="2">
-        <v>90</v>
+        <v>1.4611356146706</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -2591,13 +2610,13 @@
         <v>66</v>
       </c>
       <c r="D74" s="2">
-        <v>4000000</v>
+        <v>148.023377589456</v>
       </c>
       <c r="E74" s="2">
-        <v>4000000</v>
+        <v>90</v>
       </c>
       <c r="F74" s="2">
-        <v>4000000</v>
+        <v>90</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -2607,13 +2626,13 @@
         <v>67</v>
       </c>
       <c r="D75" s="2">
-        <v>12000000</v>
+        <v>4000000</v>
       </c>
       <c r="E75" s="2">
-        <v>13000000</v>
+        <v>4000000</v>
       </c>
       <c r="F75" s="2">
-        <v>13000000</v>
+        <v>4000000</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -2623,12 +2642,28 @@
         <v>68</v>
       </c>
       <c r="D76" s="2">
+        <v>12000000</v>
+      </c>
+      <c r="E76" s="2">
+        <v>13000000</v>
+      </c>
+      <c r="F76" s="2">
+        <v>13000000</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="5"/>
+      <c r="B77" s="7"/>
+      <c r="C77" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D77" s="2">
         <v>1</v>
       </c>
-      <c r="E76" s="2">
+      <c r="E77" s="2">
         <v>2</v>
       </c>
-      <c r="F76" s="2">
+      <c r="F77" s="2">
         <v>4</v>
       </c>
     </row>
@@ -2643,9 +2678,9 @@
     <mergeCell ref="B29:B31"/>
     <mergeCell ref="B32:B42"/>
     <mergeCell ref="A29:A42"/>
-    <mergeCell ref="B43:B56"/>
-    <mergeCell ref="B57:B76"/>
-    <mergeCell ref="A43:A76"/>
+    <mergeCell ref="B43:B57"/>
+    <mergeCell ref="B58:B77"/>
+    <mergeCell ref="A43:A77"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>